<commit_message>
Bug reports - added completion date
</commit_message>
<xml_diff>
--- a/QA_reports/bug_reports/FR10_BUG_REPORT_JV.xlsx
+++ b/QA_reports/bug_reports/FR10_BUG_REPORT_JV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtmc-my.sharepoint.com/personal/robertas_butylkinas_stud_techin_lt/Documents/Ziemos_kodas/QA_reports/bug_reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TechIN\5. Projektas\Ziemos_kodas_JV\Ziemos_kodas QA\Bug reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{2CC91818-D9DA-4415-A9C3-0378FCF5434C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23265BEF-4D20-4CB5-984D-CAF189600D22}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E530792-4166-4F09-84D9-00264DB856ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15180" yWindow="1380" windowWidth="18975" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ZK_Bug_Report" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="90">
   <si>
     <t>Field</t>
   </si>
@@ -135,6 +135,24 @@
     <t>[Additional Information or Notes]</t>
   </si>
   <si>
+    <t>Home Page</t>
+  </si>
+  <si>
+    <t>Julija Valaikiene</t>
+  </si>
+  <si>
+    <t>All three links doesn't open and doesn’t redirect user to the correct pages</t>
+  </si>
+  <si>
+    <t>Then user clicking on each link, they should open and redirect user to the correct pages.</t>
+  </si>
+  <si>
+    <t>"Navigation" section links functionality</t>
+  </si>
+  <si>
+    <t>"Navigation" section links doesn't open and doesn’t redirect user to the correct pages</t>
+  </si>
+  <si>
     <t>Windows 11, Chrome Version 119.0.6045.160</t>
   </si>
   <si>
@@ -144,36 +162,151 @@
     <t>This Bug common to mobile, tablet and mobile screens</t>
   </si>
   <si>
-    <t>BUG_ZK_FR18_3</t>
-  </si>
-  <si>
-    <t>Home Page/„app“ section</t>
-  </si>
-  <si>
-    <t>Mid</t>
-  </si>
-  <si>
-    <t>Robertas Butylkinas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">„app“ section phone image too big "Desktop"  version </t>
-  </si>
-  <si>
-    <t xml:space="preserve">in home page in "app" section on "Desktop" version "Simple UI &amp; UX" description is not to the left of the phone image </t>
-  </si>
-  <si>
-    <t>step 1: go to home page in "Desktop" version 
-step 2: scroll down to ,,app'' section
-step 3: check out description</t>
-  </si>
-  <si>
-    <t>Screenshot 2023-12-01 123829 info shuld be to the left of img</t>
-  </si>
-  <si>
-    <t>should be "Simple UI &amp; UX" on desktop version to the left of the phone picture</t>
-  </si>
-  <si>
-    <t>"Simple UI &amp; UX" is below phone picture</t>
+    <t>1.Enter the "Home" page "navigation" section. 2. Expand "hamburger" 3. Click on each link.</t>
+  </si>
+  <si>
+    <t>"Navigation" section logo functionality</t>
+  </si>
+  <si>
+    <t>"Navigation" section logo doesn't redirect user to the home page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Enter the "Home" page "navigation" section. 2. Click on the "payapi"logo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Then user clicking on the logo, located at the top left side of the webpage, it should be clickable and should redirect user to the home page. </t>
+  </si>
+  <si>
+    <t>The logo doesn't redirect user to the home page</t>
+  </si>
+  <si>
+    <t>"Navigation" section button functionality</t>
+  </si>
+  <si>
+    <t>A button doesn’t navigate user to the email schedule form.</t>
+  </si>
+  <si>
+    <t>BUG_F10_1-7</t>
+  </si>
+  <si>
+    <t>BUG_F10_1-6</t>
+  </si>
+  <si>
+    <t>Video BUG_F10_1-6.mp4</t>
+  </si>
+  <si>
+    <t>BUG_F10_1-5</t>
+  </si>
+  <si>
+    <t>Video BUG_F10_1-5.mp4</t>
+  </si>
+  <si>
+    <t>Video BUG_F10_1-7.mp4</t>
+  </si>
+  <si>
+    <t>Then user clicking on a button with the text "Schedule a Demo", it should be clickable and navigate users to the email schedule form.</t>
+  </si>
+  <si>
+    <t>1.Enter the "Home" page "navigation" section. 2. Expand the "hamburger" 3. Click on the "Shedule a Demo" button.</t>
+  </si>
+  <si>
+    <t>BUG_F10_1-8</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Designed background half-circle element is too small - need to meet design specification</t>
+  </si>
+  <si>
+    <t>Designed background half-circle element is too small</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Design should meet the requirements listed in Figma “Design System” part.</t>
+  </si>
+  <si>
+    <t>1.Enter the "Home" page "navigation" section. 2. Expand the "hamburger" 3. Check design requirements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epanded  section has text from "Home" page "api" section design </t>
+  </si>
+  <si>
+    <t>BUG_F10_1-13</t>
+  </si>
+  <si>
+    <t>BUG_F10_2-8</t>
+  </si>
+  <si>
+    <t>"Navigation" section design circle element fail</t>
+  </si>
+  <si>
+    <t>Designed background half-circle element is not by design specification</t>
+  </si>
+  <si>
+    <t>Enter the "Home" page and check "navigation" section design circle element.</t>
+  </si>
+  <si>
+    <t>Designed background half-circle element doesn’t meet design specification</t>
+  </si>
+  <si>
+    <t>Users should see a designed background half-circle element which meet design specification</t>
+  </si>
+  <si>
+    <t>BUG_F10_3-8</t>
+  </si>
+  <si>
+    <t>Users should see a designed background circle element which meet design specification</t>
+  </si>
+  <si>
+    <t>Designed background circle element doesn’t meet design specification</t>
+  </si>
+  <si>
+    <t>BUG_F10_2-8.png</t>
+  </si>
+  <si>
+    <t>BUG_F10_1-13.png</t>
+  </si>
+  <si>
+    <t>BUG_F10_1-8.pnj</t>
+  </si>
+  <si>
+    <t>BUG_F10_3-8.mp4</t>
+  </si>
+  <si>
+    <t>Windows 11, Edge Version 119.0.2151.72 (Official build) (64-bit)</t>
+  </si>
+  <si>
+    <t>BUG_F10_1-9</t>
+  </si>
+  <si>
+    <t>"Navigation" section design requirements fail</t>
+  </si>
+  <si>
+    <t>"Navigation" section design has text from other section design</t>
+  </si>
+  <si>
+    <t>All "navigation" section elements should meet design pixel perfection. The acceptable design deviation can be up to 5px.</t>
+  </si>
+  <si>
+    <t>"Navigation" section design pixel perfection acceptance fail.</t>
+  </si>
+  <si>
+    <t>All "navigation" section elements should meet design pixel perfection.</t>
+  </si>
+  <si>
+    <t>Line element doesn’t meet pixel perfection acceptance.</t>
+  </si>
+  <si>
+    <t>BUG_F10_1-9.png</t>
+  </si>
+  <si>
+    <t>1.Enter the "Home" page "navigation" section. 2. Expand the "hamburger" 3. Check design requirements "navigation" section design pixel perfection.</t>
+  </si>
+  <si>
+    <t>High</t>
   </si>
 </sst>
 </file>
@@ -183,7 +316,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,14 +352,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,12 +363,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -288,27 +409,17 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,7 +707,7 @@
   <dimension ref="A1:B179"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -619,7 +730,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -635,54 +746,52 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>37</v>
+      <c r="B5" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>37</v>
-      </c>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>38</v>
+      <c r="B7" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>39</v>
+      <c r="B8" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -691,7 +800,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -699,7 +808,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
@@ -707,7 +816,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -715,7 +824,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -723,666 +832,1232 @@
         <v>16</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="4">
+        <v>45262</v>
+      </c>
     </row>
     <row r="17" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
+      <c r="A21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="4">
+        <v>45261</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
+      <c r="A28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
+      <c r="A30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
+      <c r="A31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
+      <c r="A32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
+      <c r="A33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
+      <c r="A34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="4">
+        <v>45262</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
+      <c r="A35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
+      <c r="A37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
+      <c r="A38" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="8"/>
+      <c r="A39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="4">
+        <v>45261</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
+      <c r="A42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="3"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
+      <c r="A43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
+      <c r="A45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
+      <c r="A48" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
+      <c r="A49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
+      <c r="A51" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
+      <c r="A52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="4">
+        <v>45263</v>
+      </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="9"/>
-      <c r="B54" s="9"/>
+      <c r="A53" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
+      <c r="A55" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
+      <c r="A56" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="8"/>
+      <c r="A57" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="4">
+        <v>45261</v>
+      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="7"/>
+      <c r="A58" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="7"/>
+      <c r="A59" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
+      <c r="A60" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="3"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7"/>
+      <c r="A61" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
+      <c r="A62" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7"/>
+      <c r="A63" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7"/>
+      <c r="A64" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7"/>
+      <c r="A65" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
-      <c r="B66" s="7"/>
+      <c r="A66" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
+      <c r="A67" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7"/>
+      <c r="A68" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="7"/>
-      <c r="B69" s="7"/>
+      <c r="A69" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
+      <c r="A70" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" s="4">
+        <v>45263</v>
+      </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="7"/>
-      <c r="B71" s="7"/>
+      <c r="A71" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" s="3"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="7"/>
-      <c r="B72" s="7"/>
+      <c r="A72" s="6"/>
+      <c r="B72" s="6"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="10"/>
-      <c r="B73" s="10"/>
+      <c r="A73" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="11"/>
-      <c r="B74" s="11"/>
+      <c r="A74" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="11"/>
-      <c r="B75" s="12"/>
+      <c r="A75" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" s="8">
+        <v>45263</v>
+      </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
-      <c r="B76" s="11"/>
+      <c r="A76" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="11"/>
-      <c r="B77" s="11"/>
+      <c r="A77" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="11"/>
-      <c r="B78" s="11"/>
+      <c r="A78" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B78" s="7"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="11"/>
-      <c r="B79" s="11"/>
+      <c r="A79" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="11"/>
-      <c r="B80" s="11"/>
+      <c r="A80" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="11"/>
-      <c r="B81" s="11"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="11"/>
-      <c r="B82" s="11"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="11"/>
-      <c r="B83" s="11"/>
+      <c r="A81" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="11"/>
-      <c r="B84" s="11"/>
+      <c r="A84" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="11"/>
-      <c r="B85" s="11"/>
+      <c r="A85" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="11"/>
-      <c r="B86" s="11"/>
+      <c r="A86" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="11"/>
-      <c r="B87" s="11"/>
+      <c r="A87" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="11"/>
-      <c r="B88" s="11"/>
+      <c r="A88" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B88" s="4">
+        <v>45264</v>
+      </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="11"/>
-      <c r="B89" s="11"/>
+      <c r="A89" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B89" s="7"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="7"/>
-      <c r="B90" s="7"/>
+      <c r="A90" s="6"/>
+      <c r="B90" s="6"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="6"/>
-      <c r="B91" s="6"/>
+      <c r="A91" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="7"/>
-      <c r="B92" s="7"/>
+      <c r="A92" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="7"/>
-      <c r="B93" s="8"/>
+      <c r="A93" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B93" s="4">
+        <v>45264</v>
+      </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="7"/>
-      <c r="B94" s="7"/>
+      <c r="A94" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="7"/>
-      <c r="B95" s="7"/>
+      <c r="A95" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="7"/>
-      <c r="B96" s="7"/>
+      <c r="A96" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B96" s="3"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="7"/>
-      <c r="B97" s="7"/>
+      <c r="A97" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="7"/>
-      <c r="B98" s="7"/>
+      <c r="A98" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="7"/>
-      <c r="B99" s="7"/>
+      <c r="A99" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="7"/>
-      <c r="B100" s="7"/>
+      <c r="A100" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="7"/>
-      <c r="B101" s="7"/>
+      <c r="A101" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="7"/>
-      <c r="B102" s="7"/>
+      <c r="A102" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="7"/>
-      <c r="B103" s="7"/>
+      <c r="A103" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="7"/>
-      <c r="B104" s="7"/>
+      <c r="A104" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="7"/>
-      <c r="B105" s="7"/>
+      <c r="A105" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="7"/>
-      <c r="B106" s="7"/>
+      <c r="A106" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B106" s="4">
+        <v>45264</v>
+      </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="7"/>
-      <c r="B107" s="7"/>
+      <c r="A107" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B107" s="3"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="7"/>
-      <c r="B108" s="7"/>
+      <c r="A108" s="6"/>
+      <c r="B108" s="6"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="6"/>
-      <c r="B109" s="6"/>
+      <c r="A109" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="7"/>
-      <c r="B110" s="7"/>
+      <c r="A110" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="7"/>
-      <c r="B111" s="8"/>
+      <c r="A111" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111" s="4">
+        <v>45263</v>
+      </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="7"/>
-      <c r="B112" s="7"/>
+      <c r="A112" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="7"/>
-      <c r="B113" s="7"/>
+      <c r="A113" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="7"/>
-      <c r="B114" s="7"/>
+      <c r="A114" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B114" s="3"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="7"/>
-      <c r="B115" s="7"/>
+      <c r="A115" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="7"/>
-      <c r="B116" s="7"/>
+      <c r="A116" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="7"/>
-      <c r="B117" s="7"/>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="7"/>
-      <c r="B118" s="7"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="7"/>
-      <c r="B119" s="7"/>
+      <c r="A117" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="7"/>
-      <c r="B120" s="7"/>
+      <c r="A120" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="7"/>
-      <c r="B121" s="7"/>
+      <c r="A121" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="7"/>
-      <c r="B122" s="7"/>
+      <c r="A122" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="7"/>
-      <c r="B123" s="7"/>
+      <c r="A123" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="7"/>
-      <c r="B124" s="7"/>
+      <c r="A124" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B124" s="4">
+        <v>45264</v>
+      </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="7"/>
-      <c r="B125" s="7"/>
+      <c r="A125" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B125" s="3"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="7"/>
-      <c r="B126" s="7"/>
+      <c r="A126" s="6"/>
+      <c r="B126" s="6"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="6"/>
-      <c r="B127" s="6"/>
+      <c r="A127" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="7"/>
-      <c r="B128" s="7"/>
+      <c r="A128" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="7"/>
-      <c r="B129" s="8"/>
+      <c r="A129" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B129" s="4">
+        <v>45263</v>
+      </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="7"/>
-      <c r="B130" s="7"/>
+      <c r="A130" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="7"/>
-      <c r="B131" s="7"/>
+      <c r="A131" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="7"/>
-      <c r="B132" s="7"/>
+      <c r="A132" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B132" s="3"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="7"/>
-      <c r="B133" s="7"/>
+      <c r="A133" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="7"/>
-      <c r="B134" s="7"/>
+      <c r="A134" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="7"/>
-      <c r="B135" s="7"/>
+      <c r="A135" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="7"/>
-      <c r="B136" s="7"/>
+      <c r="A136" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="7"/>
-      <c r="B137" s="7"/>
+      <c r="A137" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="7"/>
-      <c r="B138" s="7"/>
+      <c r="A138" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="7"/>
-      <c r="B139" s="7"/>
+      <c r="A139" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="7"/>
-      <c r="B140" s="7"/>
+      <c r="A140" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="7"/>
-      <c r="B141" s="7"/>
+      <c r="A141" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="7"/>
-      <c r="B142" s="7"/>
+      <c r="A142" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B142" s="4">
+        <v>45264</v>
+      </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="7"/>
-      <c r="B143" s="7"/>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="9"/>
-      <c r="B144" s="9"/>
+      <c r="A143" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B143" s="3"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="6"/>
-      <c r="B145" s="6"/>
+      <c r="A145" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="7"/>
-      <c r="B146" s="7"/>
+      <c r="A146" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="7"/>
-      <c r="B147" s="8"/>
+      <c r="A147" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B147" s="4">
+        <v>45263</v>
+      </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="7"/>
-      <c r="B148" s="7"/>
+      <c r="A148" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="7"/>
-      <c r="B149" s="7"/>
+      <c r="A149" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="7"/>
-      <c r="B150" s="7"/>
+      <c r="A150" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B150" s="3"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="7"/>
-      <c r="B151" s="7"/>
+      <c r="A151" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="7"/>
-      <c r="B152" s="7"/>
+      <c r="A152" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="7"/>
-      <c r="B153" s="7"/>
+      <c r="A153" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="7"/>
-      <c r="B154" s="7"/>
+      <c r="A154" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="7"/>
-      <c r="B155" s="7"/>
+      <c r="A155" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="7"/>
-      <c r="B156" s="7"/>
+      <c r="A156" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="7"/>
-      <c r="B157" s="7"/>
+      <c r="A157" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="7"/>
-      <c r="B158" s="7"/>
+      <c r="A158" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="7"/>
-      <c r="B159" s="7"/>
+      <c r="A159" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="7"/>
-      <c r="B160" s="7"/>
+      <c r="A160" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B160" s="4">
+        <v>45264</v>
+      </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="7"/>
-      <c r="B161" s="7"/>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="9"/>
-      <c r="B162" s="9"/>
+      <c r="A161" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B161" s="3"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="6"/>
-      <c r="B163" s="6"/>
+      <c r="A163" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="7"/>
-      <c r="B164" s="7"/>
+      <c r="A164" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="7"/>
-      <c r="B165" s="8"/>
+      <c r="A165" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B165" s="4">
+        <v>45263</v>
+      </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="7"/>
-      <c r="B166" s="7"/>
+      <c r="A166" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="7"/>
-      <c r="B167" s="7"/>
+      <c r="A167" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="7"/>
-      <c r="B168" s="7"/>
+      <c r="A168" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B168" s="3"/>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="7"/>
-      <c r="B169" s="7"/>
+      <c r="A169" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="7"/>
-      <c r="B170" s="7"/>
+      <c r="A170" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="7"/>
-      <c r="B171" s="7"/>
+      <c r="A171" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="7"/>
-      <c r="B172" s="7"/>
+      <c r="A172" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="7"/>
-      <c r="B173" s="7"/>
+      <c r="A173" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="7"/>
-      <c r="B174" s="7"/>
+      <c r="A174" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="7"/>
-      <c r="B175" s="7"/>
+      <c r="A175" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="7"/>
-      <c r="B176" s="7"/>
+      <c r="A176" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="7"/>
-      <c r="B177" s="7"/>
+      <c r="A177" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="7"/>
-      <c r="B178" s="7"/>
+      <c r="A178" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B178" s="4">
+        <v>45264</v>
+      </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="7"/>
-      <c r="B179" s="7"/>
+      <c r="A179" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B179" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1396,7 +2071,7 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView zoomScale="23" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>